<commit_message>
Added a Materials Category filter to the quotation html and quotation js. Added new materials to the quotes database
</commit_message>
<xml_diff>
--- a/data/quotes.xlsx
+++ b/data/quotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UOTSTD690\Documents\Year 2 (2025)\Internet Programming I (CS222)\Projects\Supplier_Dashboard_Web_Application\Supplier_Dashboard_web_Application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BBD27E7-A2DB-40AB-A1ED-38A7BF40830E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E418F089-CCCA-47BB-AC10-B49BA7B8F29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9768" yWindow="0" windowWidth="13368" windowHeight="12336" xr2:uid="{E8A72D2A-36DB-46B3-8451-87814F61D33C}"/>
+    <workbookView xWindow="8496" yWindow="0" windowWidth="14640" windowHeight="12336" xr2:uid="{E8A72D2A-36DB-46B3-8451-87814F61D33C}"/>
   </bookViews>
   <sheets>
     <sheet name="quotes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="141">
   <si>
     <t>SUPPLIER</t>
   </si>
@@ -343,6 +343,122 @@
   </si>
   <si>
     <t>Screw Stitch C3 PHL 8-15x25 PBX100 #CBZ7425</t>
+  </si>
+  <si>
+    <t>Lus</t>
+  </si>
+  <si>
+    <t>CABLE CIRC 1C 300mm BK XLPE NAN XSD300CLVNB 500M Cu 0.6/1kV</t>
+  </si>
+  <si>
+    <t>LUG CABLE CU 300mm2 BLANK CABAC CAL300 CAL300BM - 5pack</t>
+  </si>
+  <si>
+    <t>HEATSHRINK 38-19mm BL CABAC XLP38BL/4FT 1.2M LENGTH</t>
+  </si>
+  <si>
+    <t>HEATSHRINK 38-19mm G/Y CABAC XLP38YG/4FT 1.2M LENGTH</t>
+  </si>
+  <si>
+    <t>HEATSHRINK 38-19mm RD CABAC XLP38RD/4FT 1.2M LENGTH</t>
+  </si>
+  <si>
+    <t>HEATSHRINK 38-19mm WH CABAC XLP38WH/4FT 1.2M LENGTH</t>
+  </si>
+  <si>
+    <t>CONDUIT RIGID HD 150mmX4M OR 150HDCON-GEN</t>
+  </si>
+  <si>
+    <t>BEND SWEEP 90DEG 150mm HD OR BS15090HDOR-GEN</t>
+  </si>
+  <si>
+    <t>LUG CABLE CU 95mm2XM10 HOLE CABAC CAL95-10</t>
+  </si>
+  <si>
+    <t>CABLE B/WIRE 1C 95mm G/Y OLEX BAAC22A5001AAHN 500M 0.6/1kV</t>
+  </si>
+  <si>
+    <t>CONDUIT RIGID HD 32mmX4M OR 32HDCON-GEN HEAVY DUTY UNDERGROUND</t>
+  </si>
+  <si>
+    <t>BEND SWEEP 90DEG 32mm HD OR BS3290HDOR-GEN U/G ORANGE</t>
+  </si>
+  <si>
+    <t>EARTH ROD 19mm X 1.8M TRANSNET CTNCER1918 PPL 142001</t>
+  </si>
+  <si>
+    <t>EARTH CLAMP 13-15mm 16-120mm2 TRANSNET CTNEC-210 1 CABLE</t>
+  </si>
+  <si>
+    <t>LUG CABLE CU 35mm2XM8 HOLE CABAC CAL35-8 50/BOX</t>
+  </si>
+  <si>
+    <t>LUG CABLE CU 6mm2XM8 HOLE CABAC CAL6-8 100/BOX</t>
+  </si>
+  <si>
+    <t>CABLE GLAND 40mm NYLON CABAC GN40 OD19-28MM - 5/BOX</t>
+  </si>
+  <si>
+    <t>CABLE GLAND 20mm NYLON CABAC GN20 OD 8-13MM 25/BOX</t>
+  </si>
+  <si>
+    <t>BATTEN LED 35W EMERGENCY SLIM DAVIS ACS435CTEMS 4FT DIFF 3000K-6000K 50,000HRS</t>
+  </si>
+  <si>
+    <t>SURFACE SOCKET 3PIN 10A SINGLE EVO PB1L</t>
+  </si>
+  <si>
+    <t>JUNCTION BOX 3WY 20mm SHLW PVC JBS3W20PVC-GEN CONDUIT
+FITTING</t>
+  </si>
+  <si>
+    <t>HOLE SAW METAL 20mm CABAC HS20 HIGH SPEED 20mm</t>
+  </si>
+  <si>
+    <t>HOLE SAW 25mm METAL H/SPEED CABAC HS25</t>
+  </si>
+  <si>
+    <t>HOLE SAW 32mm METAL H/S 1.1/4 CABAC HS32</t>
+  </si>
+  <si>
+    <t>HOLE SAW 40mm INDUST CABAC HS40 602682</t>
+  </si>
+  <si>
+    <t>HOLE SAW 51mm INDUST HS CABAC HS51</t>
+  </si>
+  <si>
+    <t>FLOODLIGHT LED 100W 6500K VAC LK SIGMA LF-SL03 100W 10000lm IP65 CABLE0.3M LFST100</t>
+  </si>
+  <si>
+    <t>LINK 7 HOLE 100A NEUTRAL BK TESLA NL7</t>
+  </si>
+  <si>
+    <t>SADDLE HALF 20mm ZINC PLATED HS20ZP-GEN</t>
+  </si>
+  <si>
+    <t>CONDUIT RIGID MD 20mmX4M GY 20MDCON-GEN PPL 171046</t>
+  </si>
+  <si>
+    <t>BEND 90DEG 20mm PVC GY B2090GY-GEN CONDUIT FITTING</t>
+  </si>
+  <si>
+    <t>BENDING SPRING 20mm WATTMASTER WATCB20 FOR HD CONDUIT</t>
+  </si>
+  <si>
+    <t>BENDING SPRING 25mm WATTMASTER WATCB25 FOR HD CONDUIT</t>
+  </si>
+  <si>
+    <t>CONNECTOR 32A TWIN SCREW CABAC C32A2 (SOLD LOOSE) 50/pack</t>
+  </si>
+  <si>
+    <t>ADAPTABLE BOX 108x108x76mm AB10810876-GEN</t>
+  </si>
+  <si>
+    <t>DUCT PVC 75X75mm 4M WHITE CD7575WH-GEN</t>
+  </si>
+  <si>
+    <t>ISOLATOR SWITCH 1P 32A LARGE TESLA TWIS1P32L WEATHER PROOF
+IP56</t>
   </si>
 </sst>
 </file>
@@ -385,18 +501,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -713,1175 +830,1838 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FC0569-8C4B-48DA-BCC4-8AE4D3A126F6}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="17.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2">
         <v>2239.9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>2199.9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2">
         <v>229.9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>36.9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2">
         <v>19.899999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2">
         <v>11.95</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2">
         <v>5.9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2">
         <v>28.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>64.900000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>695</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
         <v>129.94999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>99.9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
         <v>219.9</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
         <v>149.9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
         <v>139.9</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>319408</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>314479</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
         <v>45.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>601564</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
         <v>420</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>601514</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="2">
         <v>396</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>601323</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2">
         <v>928</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>604044</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2">
         <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>604277</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2">
         <v>28.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>604350</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2">
         <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>604626</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2">
         <v>28.5</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>605767</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2">
         <v>1490</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>607501</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2">
         <v>2767</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>602620</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2">
         <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>604235</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2">
         <v>576</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>600694</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2">
         <v>360</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>607384</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2">
         <v>730</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>600927</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2">
         <v>608</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>607140</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2">
         <v>47.11</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>1020051</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="2">
         <v>49.95</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>2355031</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="2">
         <v>159.9</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>2355332</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="1">
+      <c r="D36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2">
         <v>38.5</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>1464014</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="2">
         <v>64.73</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>1464014</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2">
         <v>64.73</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="1">
+      <c r="A39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="2">
         <v>118386</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="D39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="2">
         <v>97.73</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="1">
+      <c r="A40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="2">
         <v>115129</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="1">
+      <c r="D40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2">
         <v>1.82</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="1">
+      <c r="A41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2">
         <v>103986</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="2">
         <v>5.45</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="1">
+      <c r="A42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="2">
         <v>114246</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="D42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="2">
         <v>1.36</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="1">
+      <c r="A43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="2">
         <v>123088</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="1">
+      <c r="D43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="2">
         <v>37.270000000000003</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="1">
+      <c r="A44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="2">
         <v>103856</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="1">
+      <c r="D44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="1">
+      <c r="A45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="2">
         <v>107925</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="1">
+      <c r="D45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="2">
         <v>79.55</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="1">
+      <c r="A46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="2">
         <v>114380</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="1">
+      <c r="D46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="2">
         <v>9.09</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47" s="1">
+      <c r="A47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="2">
         <v>118068</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="1">
+      <c r="D47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="2">
         <v>40.909999999999997</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>6070201</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="1">
+      <c r="D48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2">
         <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>6020629</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="1">
+      <c r="D49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="2">
         <v>108.18</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>6020099</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="1">
+      <c r="D50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="2">
         <v>388.18</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>6040720</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="1">
+      <c r="D51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="2">
         <v>60.72</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>3020333</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="2">
         <v>10.95</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>1080717</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="2">
         <v>47.64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>8010215</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="1">
+      <c r="D54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="2">
         <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>5082122</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="1">
+      <c r="D55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="2">
         <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>2010517</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="2">
         <v>299.08999999999997</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="2">
         <v>1030438</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="2">
         <v>318.18</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="2">
         <v>5031193</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="1">
+      <c r="D58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="2">
         <v>31.82</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="2">
         <v>3030443</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="1">
+      <c r="D59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="2">
         <v>3.18</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="2">
         <v>2010508</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="2">
         <v>145.44999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="2">
         <v>10090015</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="2">
         <v>54.55</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="2">
         <v>10090015</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="2">
         <v>54.55</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="2">
         <v>3040191</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="1">
+      <c r="D63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="2">
         <v>75.41</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="2">
         <v>11099511</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="1">
+      <c r="D64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="2">
         <v>2.73</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="2">
         <v>8010154</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="1">
+      <c r="D65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="2">
         <v>3.73</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="2">
         <v>8400646</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="1">
+      <c r="D66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="2">
         <v>15.45</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="2">
         <v>6050512</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="1">
+      <c r="D67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="2">
         <v>3.63</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="2">
         <v>3040442</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="1">
+      <c r="D68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="2">
         <v>20.56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2">
+        <v>113754</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E69" s="2">
+        <v>235.23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2">
+        <v>102957</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E70" s="2">
+        <v>88.64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="2">
+        <v>104059</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="2">
+        <v>33.409999999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="2">
+        <v>104060</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="2">
+        <v>42.62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73" s="2">
+        <v>104061</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="2">
+        <v>33.409999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="2">
+        <v>104062</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="2">
+        <v>33.409999999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75" s="2">
+        <v>118193</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2">
+        <v>385.91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="2">
+        <v>118190</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="2">
+        <v>606.82000000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="2">
+        <v>102995</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E77" s="2">
+        <v>17.05</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" s="2">
+        <v>101943</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" s="2">
+        <v>92.05</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="2">
+        <v>115121</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="2">
+        <v>27.27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="2">
+        <v>114330</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="2">
+        <v>12.27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81" s="2">
+        <v>105314</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="2">
+        <v>167.05</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="2">
+        <v>103426</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="2">
+        <v>30.68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="2">
+        <v>102963</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="2">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" s="2">
+        <v>102985</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E84" s="2">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B85" s="2">
+        <v>102172</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E85" s="2">
+        <v>30.91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86" s="2">
+        <v>102169</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E86" s="2">
+        <v>7.82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B87" s="2">
+        <v>120316</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="2">
+        <v>613.64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="2">
+        <v>123474</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="2">
+        <v>9.5500000000000007</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B89" s="2">
+        <v>114380</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="2">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B90" s="2">
+        <v>114246</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B91" s="2">
+        <v>100840</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="2">
+        <v>56.36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B92" s="2">
+        <v>100842</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="2">
+        <v>52.73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" s="2">
+        <v>100844</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="2">
+        <v>65.91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B94" s="2">
+        <v>100845</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95" s="2">
+        <v>100846</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="2">
+        <v>88.64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B96" s="2">
+        <v>121372</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="2">
+        <v>271.82</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B97" s="2">
+        <v>102886</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="2">
+        <v>19.09</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B98" s="2">
+        <v>118198</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B99" s="2">
+        <v>118079</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="2">
+        <v>17.27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B100" s="2">
+        <v>114386</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="2">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B101" s="2">
+        <v>114356</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="2">
+        <v>145.44999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B102" s="2">
+        <v>114357</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="2">
+        <v>195.45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B103" s="2">
+        <v>103295</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="2">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B104" s="2">
+        <v>118330</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="2">
+        <v>25.91</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B105" s="2">
+        <v>121385</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="2">
+        <v>59.09</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106" s="2">
+        <v>118805</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="2">
+        <v>68.180000000000007</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B107" s="2">
+        <v>118079</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="2">
+        <v>17.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>